<commit_message>
new patient gui + load image
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
   <si>
     <t>Hours</t>
   </si>
@@ -174,9 +174,6 @@
     <t>اسفند 98 تا خرداد 99</t>
   </si>
   <si>
-    <t>تیر 99 تا شهریور 99</t>
-  </si>
-  <si>
     <t>* Multithreading</t>
   </si>
   <si>
@@ -235,6 +232,15 @@
   </si>
   <si>
     <t>• Segmentation (Lung/Airway)         (not integrated)</t>
+  </si>
+  <si>
+    <t>تیر 99</t>
+  </si>
+  <si>
+    <t>مرداد 99</t>
+  </si>
+  <si>
+    <t>* Database</t>
   </si>
 </sst>
 </file>
@@ -849,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I100"/>
+  <dimension ref="A2:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,8 +902,8 @@
         <v>4</v>
       </c>
       <c r="I4" s="41">
-        <f>C11+C22+C34+C45+C57+C72+C83+C98</f>
-        <v>264</v>
+        <f>C11+C22+C34+C45+C57+C72+C83+C98+C112</f>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1450,7 +1456,7 @@
         <v>5</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -1461,7 +1467,7 @@
         <v>7</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -1472,7 +1478,7 @@
         <v>5</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -1483,7 +1489,7 @@
         <v>7</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -1583,35 +1589,35 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C79" s="2">
         <v>7</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C80" s="2">
         <v>3</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -1624,7 +1630,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C82" s="2">
         <v>2</v>
@@ -1673,7 +1679,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="25" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>10</v>
@@ -1687,24 +1693,24 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C90" s="2">
         <v>4</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -1715,7 +1721,7 @@
         <v>9</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -1726,12 +1732,12 @@
         <v>6</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C93" s="2">
         <v>2</v>
@@ -1747,7 +1753,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C95" s="2">
         <v>3</v>
@@ -1755,21 +1761,21 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C96" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C97" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B98" s="18" t="s">
         <v>4</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C99" s="4" t="s">
         <v>2</v>
       </c>
@@ -1786,13 +1792,121 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C100" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D100" s="21">
         <f>C98</f>
         <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="36"/>
+      <c r="B103" s="36"/>
+      <c r="C103" s="36"/>
+      <c r="D103" s="36"/>
+      <c r="E103" s="36"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B105" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C105" s="2"/>
+      <c r="E105" s="39"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B106" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="E106" s="11"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B107" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="E107" s="11"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B108" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C108" s="2">
+        <v>2</v>
+      </c>
+      <c r="E108" s="11"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B109" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C109" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B110" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C110" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B111" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C111" s="2"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B112" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" s="19">
+        <f>SUM(C105:C111)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C113" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C114" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="21">
+        <f>C112</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
patient tab completed for now
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
   <si>
     <t>Hours</t>
   </si>
@@ -867,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I112"/>
+  <dimension ref="A2:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,8 +914,8 @@
         <v>4</v>
       </c>
       <c r="I4" s="41">
-        <f>C11+C22+C34+C45+C57+C72+C83+C98+C110</f>
-        <v>276</v>
+        <f>C11+C22+C34+C45+C57+C72+C83+C98+C111</f>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1848,7 +1848,7 @@
         <v>73</v>
       </c>
       <c r="C105" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E105" s="39" t="s">
         <v>77</v>
@@ -1883,34 +1883,43 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" s="2">
+        <v>2</v>
+      </c>
+      <c r="E109" s="35"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B110" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B110" s="18" t="s">
+      <c r="C110" s="2"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B111" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C110" s="19">
-        <f>SUM(C105:C109)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C111" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D111" s="3">
-        <v>0</v>
+      <c r="C111" s="19">
+        <f>SUM(C105:C110)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C112" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C113" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D112" s="21">
-        <f>C110</f>
-        <v>12</v>
+      <c r="D113" s="21">
+        <f>C111</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
online registration matrix added
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -870,7 +870,7 @@
   <dimension ref="A2:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +915,7 @@
       </c>
       <c r="I4" s="41">
         <f>C11+C22+C34+C45+C57+C72+C83+C98+C111</f>
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1886,7 +1886,7 @@
         <v>43</v>
       </c>
       <c r="C109" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E109" s="35"/>
     </row>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="C111" s="19">
         <f>SUM(C105:C110)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="D113" s="21">
         <f>C111</f>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
online is matched with offline
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
   <si>
     <t>Hours</t>
   </si>
@@ -240,19 +240,13 @@
     <t>مرداد 99</t>
   </si>
   <si>
-    <t>* Tab Patients</t>
-  </si>
-  <si>
-    <t>* Tab View</t>
-  </si>
-  <si>
-    <t>* Tab Process</t>
-  </si>
-  <si>
-    <t>* Tab Tracking</t>
-  </si>
-  <si>
     <t>• Patients Database</t>
+  </si>
+  <si>
+    <t>* Patients Database</t>
+  </si>
+  <si>
+    <t>* Other</t>
   </si>
 </sst>
 </file>
@@ -867,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I113"/>
+  <dimension ref="A2:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,8 +908,8 @@
         <v>4</v>
       </c>
       <c r="I4" s="41">
-        <f>C11+C22+C34+C45+C57+C72+C83+C98+C111</f>
-        <v>283</v>
+        <f>C11+C22+C34+C45+C57+C72+C83+C98+C109</f>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1845,81 +1839,66 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C105" s="2">
         <v>9</v>
       </c>
       <c r="E105" s="39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C106" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E106" s="11"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C107" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E107" s="11"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C108" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B109" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" s="19">
+        <f>SUM(C105:C108)</f>
+        <v>35</v>
+      </c>
+      <c r="E109" s="35"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C110" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C111" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E108" s="11"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B109" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C109" s="2">
-        <v>5</v>
-      </c>
-      <c r="E109" s="35"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B110" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B111" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C111" s="19">
-        <f>SUM(C105:C110)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C112" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D112" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C113" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D113" s="21">
-        <f>C111</f>
-        <v>19</v>
+      <c r="D111" s="21">
+        <f>C109-D110</f>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start refactoring (separating files)
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="81">
   <si>
     <t>Hours</t>
   </si>
@@ -246,9 +246,6 @@
     <t>* Patients Database</t>
   </si>
   <si>
-    <t>* Other</t>
-  </si>
-  <si>
     <t>* Online Tracking</t>
   </si>
   <si>
@@ -256,6 +253,15 @@
   </si>
   <si>
     <t>• Total Payments</t>
+  </si>
+  <si>
+    <t>* Meetings &amp; other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• </t>
+  </si>
+  <si>
+    <t>شهریور و مهر 99</t>
   </si>
 </sst>
 </file>
@@ -874,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I112"/>
+  <dimension ref="A2:I123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,7 +928,7 @@
       </c>
       <c r="I4" s="41">
         <f>C11+C22+C34+C45+C57+C72+C83+C98+C110</f>
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -940,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5" s="43">
         <f>E11+E22+E34+E45+E57+E72+E83+E98</f>
@@ -1908,7 +1914,7 @@
         <v>6</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -1918,19 +1924,18 @@
       <c r="C107" s="2">
         <v>15</v>
       </c>
-      <c r="E107" s="11"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C108" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C109" s="2">
         <v>5</v>
@@ -1943,11 +1948,11 @@
       </c>
       <c r="C110" s="19">
         <f>SUM(C105:C109)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E110" s="42">
         <f>C110*40000</f>
-        <v>1520000</v>
+        <v>1600000</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -1964,7 +1969,108 @@
       </c>
       <c r="D112" s="21">
         <f>C110-D111</f>
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="36"/>
+      <c r="B114" s="36"/>
+      <c r="C114" s="36"/>
+      <c r="D114" s="36"/>
+      <c r="E114" s="36"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B116" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" s="2">
+        <v>1</v>
+      </c>
+      <c r="E116" s="39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B117" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C117" s="2">
+        <v>2</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B118" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C118" s="2"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B119" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C119" s="2"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B120" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C120" s="2"/>
+      <c r="E120" s="35"/>
+    </row>
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B121" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" s="19">
+        <f>SUM(C116:C120)</f>
+        <v>3</v>
+      </c>
+      <c r="E121" s="42">
+        <f>C121*40000</f>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C122" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C123" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D123" s="21">
+        <f>C121-D122</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename vars and funcs to snake case
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -246,9 +246,6 @@
     <t>* Patients Database</t>
   </si>
   <si>
-    <t>* Online Tracking</t>
-  </si>
-  <si>
     <t>• Online Tracking (Registered)</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>شهریور و مهر 99</t>
+  </si>
+  <si>
+    <t>* Tracker</t>
   </si>
 </sst>
 </file>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" s="43">
         <f>E11+E22+E34+E45+E57+E72+E83+E98</f>
@@ -1914,7 +1914,7 @@
         <v>6</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -1927,7 +1927,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C108" s="2">
         <v>5</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C109" s="2">
         <v>5</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>10</v>
@@ -2007,10 +2007,10 @@
         <v>52</v>
       </c>
       <c r="C116" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E116" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -2021,7 +2021,7 @@
         <v>2</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -2032,13 +2032,15 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C119" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="C119" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C120" s="2">
         <v>1</v>
@@ -2051,11 +2053,11 @@
       </c>
       <c r="C121" s="19">
         <f>SUM(C116:C120)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E121" s="42">
         <f>C121*40000</f>
-        <v>320000</v>
+        <v>440000</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -2072,7 +2074,7 @@
       </c>
       <c r="D123" s="21">
         <f>C121-D122</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted for the phantom (3D widget + 2D views)
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
   <si>
     <t>Hours</t>
   </si>
@@ -255,13 +255,16 @@
     <t>* Meetings &amp; other</t>
   </si>
   <si>
-    <t xml:space="preserve">• </t>
-  </si>
-  <si>
     <t>شهریور و مهر 99</t>
   </si>
   <si>
     <t>* Tracker</t>
+  </si>
+  <si>
+    <t>• Adjusted orientstion widget for the phantom</t>
+  </si>
+  <si>
+    <t>• Adjusted 2D views for the phantom</t>
   </si>
 </sst>
 </file>
@@ -880,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I123"/>
+  <dimension ref="A2:I124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1927,7 +1930,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C108" s="2">
         <v>5</v>
@@ -1990,7 +1993,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>10</v>
@@ -2010,7 +2013,7 @@
         <v>6</v>
       </c>
       <c r="E116" s="39" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -2021,7 +2024,7 @@
         <v>2</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -2032,7 +2035,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C119" s="2">
         <v>2</v>
@@ -2040,29 +2043,32 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C120" s="2">
+        <v>2</v>
+      </c>
+      <c r="E120" s="35"/>
+    </row>
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B121" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C120" s="2">
+      <c r="C121" s="2">
         <v>1</v>
       </c>
-      <c r="E120" s="35"/>
-    </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B121" s="18" t="s">
+      <c r="E121" s="42">
+        <f>C122*40000</f>
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B122" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C121" s="19">
-        <f>SUM(C116:C120)</f>
-        <v>11</v>
-      </c>
-      <c r="E121" s="42">
-        <f>C121*40000</f>
-        <v>440000</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C122" s="4" t="s">
-        <v>2</v>
+      <c r="C122" s="19">
+        <f>SUM(C116:C121)</f>
+        <v>13</v>
       </c>
       <c r="D122" s="3">
         <v>0</v>
@@ -2070,11 +2076,16 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C123" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D123" s="21">
+        <f>C122-D122</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C124" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="D123" s="21">
-        <f>C121-D122</f>
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
read points and centerline organized
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -886,7 +886,7 @@
   <dimension ref="A2:I124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2021,7 +2021,7 @@
         <v>47</v>
       </c>
       <c r="C117" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>81</v>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="E121" s="42">
         <f>C122*40000</f>
-        <v>520000</v>
+        <v>560000</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="C122" s="19">
         <f>SUM(C116:C121)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D122" s="3">
         <v>0</v>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="D123" s="21">
         <f>C122-D122</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
registration ui + some codes
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -255,9 +255,6 @@
     <t>* Meetings &amp; other</t>
   </si>
   <si>
-    <t>شهریور و مهر 99</t>
-  </si>
-  <si>
     <t>* Tracker</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>• Adjusted 2D views for the phantom</t>
+  </si>
+  <si>
+    <t>شهریور، مهر و آبان 99</t>
   </si>
 </sst>
 </file>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1885,7 +1885,7 @@
       <c r="E103" s="36"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="25" t="s">
+      <c r="A104" s="32" t="s">
         <v>72</v>
       </c>
       <c r="B104" s="7" t="s">
@@ -1930,7 +1930,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C108" s="2">
         <v>5</v>
@@ -1946,10 +1946,10 @@
       <c r="E109" s="35"/>
     </row>
     <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B110" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C110" s="19">
+      <c r="B110" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" s="34">
         <f>SUM(C105:C109)</f>
         <v>40</v>
       </c>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>10</v>
@@ -2013,7 +2013,7 @@
         <v>6</v>
       </c>
       <c r="E116" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -2021,21 +2021,23 @@
         <v>47</v>
       </c>
       <c r="C117" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B118" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C118" s="2"/>
+      <c r="C118" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C119" s="2">
         <v>2</v>
@@ -2059,7 +2061,7 @@
       </c>
       <c r="E121" s="42">
         <f>C122*40000</f>
-        <v>560000</v>
+        <v>760000</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -2068,7 +2070,7 @@
       </c>
       <c r="C122" s="19">
         <f>SUM(C116:C121)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D122" s="3">
         <v>0</v>
@@ -2080,7 +2082,7 @@
       </c>
       <c r="D123" s="21">
         <f>C122-D122</f>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
load image centerline + db update completed
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
   <si>
     <t>Hours</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>شهریور، مهر و آبان 99</t>
+  </si>
+  <si>
+    <t>• Extract/Load Image Centerline</t>
   </si>
 </sst>
 </file>
@@ -883,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I124"/>
+  <dimension ref="A2:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,8 +933,8 @@
         <v>4</v>
       </c>
       <c r="I4" s="41">
-        <f>C11+C22+C34+C45+C57+C72+C83+C98+C110</f>
-        <v>304</v>
+        <f>C11+C22+C34+C45+C57+C72+C83+C98+C110+C123</f>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2021,7 +2024,7 @@
         <v>47</v>
       </c>
       <c r="C117" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>80</v>
@@ -2032,7 +2035,10 @@
         <v>43</v>
       </c>
       <c r="C118" s="2">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -2054,40 +2060,48 @@
     </row>
     <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C121" s="2">
         <v>1</v>
       </c>
       <c r="E121" s="42">
-        <f>C122*40000</f>
-        <v>760000</v>
+        <f>C123*40000</f>
+        <v>960000</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C122" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B123" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C122" s="19">
-        <f>SUM(C116:C121)</f>
-        <v>19</v>
-      </c>
-      <c r="D122" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C123" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D123" s="21">
-        <f>C122-D122</f>
-        <v>19</v>
+      <c r="C123" s="19">
+        <f>SUM(C116:C122)</f>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C124" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C125" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="D125" s="21">
+        <f>C123-D124</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save and load tracker centerline in prep tab
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -502,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -605,6 +605,7 @@
     <xf numFmtId="3" fontId="12" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -889,7 +890,7 @@
   <dimension ref="A2:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,7 +935,7 @@
       </c>
       <c r="I4" s="41">
         <f>C11+C22+C34+C45+C57+C72+C83+C98+C110+C123</f>
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -2035,7 +2036,7 @@
         <v>43</v>
       </c>
       <c r="C118" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E118" s="11" t="s">
         <v>82</v>
@@ -2067,7 +2068,7 @@
       </c>
       <c r="E121" s="42">
         <f>C123*40000</f>
-        <v>1000000</v>
+        <v>1160000</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -2077,6 +2078,10 @@
       <c r="C122" s="2">
         <v>2</v>
       </c>
+      <c r="E122" s="44">
+        <f>E121-700000</f>
+        <v>460000</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B123" s="18" t="s">
@@ -2084,7 +2089,7 @@
       </c>
       <c r="C123" s="19">
         <f>SUM(C116:C122)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -2101,7 +2106,7 @@
       </c>
       <c r="D125" s="21">
         <f>C123-D124</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated timesheet for 6,7,8 of 1399
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
   <si>
     <t>Hours</t>
   </si>
@@ -258,9 +258,6 @@
     <t>* Tracker</t>
   </si>
   <si>
-    <t>• Adjusted orientstion widget for the phantom</t>
-  </si>
-  <si>
     <t>• Adjusted 2D views for the phantom</t>
   </si>
   <si>
@@ -268,6 +265,15 @@
   </si>
   <si>
     <t>• Extract/Load Image Centerline</t>
+  </si>
+  <si>
+    <t>• Adjusted orientation widget for the phantom</t>
+  </si>
+  <si>
+    <t>• Integrated Registration Process</t>
+  </si>
+  <si>
+    <t>• Record/Load Tracker Centerline</t>
   </si>
 </sst>
 </file>
@@ -502,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -605,7 +611,6 @@
     <xf numFmtId="3" fontId="12" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -889,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,7 +940,7 @@
       </c>
       <c r="I4" s="41">
         <f>C11+C22+C34+C45+C57+C72+C83+C98+C110+C123</f>
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -956,8 +961,8 @@
         <v>76</v>
       </c>
       <c r="I5" s="43">
-        <f>E11+E22+E34+E45+E57+E72+E83+E98</f>
-        <v>8030000</v>
+        <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122</f>
+        <v>11030000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1997,7 +2002,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>10</v>
@@ -2017,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="E116" s="39" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -2025,10 +2030,10 @@
         <v>47</v>
       </c>
       <c r="C117" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -2039,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -2049,6 +2054,9 @@
       <c r="C119" s="2">
         <v>2</v>
       </c>
+      <c r="E119" s="11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
@@ -2057,30 +2065,28 @@
       <c r="C120" s="2">
         <v>2</v>
       </c>
-      <c r="E120" s="35"/>
-    </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E120" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C121" s="2">
         <v>1</v>
       </c>
-      <c r="E121" s="42">
-        <f>C123*40000</f>
-        <v>1280000</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C122" s="2">
         <v>2</v>
       </c>
-      <c r="E122" s="44">
-        <f>E121-700000</f>
-        <v>580000</v>
+      <c r="E122" s="42">
+        <f>C123*40000</f>
+        <v>1400000</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -2089,7 +2095,7 @@
       </c>
       <c r="C123" s="19">
         <f>SUM(C116:C122)</f>
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -2106,7 +2112,7 @@
       </c>
       <c r="D125" s="21">
         <f>C123-D124</f>
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tracker crashes fixed + splash messages
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="88">
   <si>
     <t>Hours</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>• Record/Load Tracker Centerline</t>
+  </si>
+  <si>
+    <t>آذر 99</t>
+  </si>
+  <si>
+    <t>• Fix tracker's crash</t>
+  </si>
+  <si>
+    <t>• Added tracker status messages</t>
   </si>
 </sst>
 </file>
@@ -892,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I125"/>
+  <dimension ref="A2:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114:E125"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,8 +970,8 @@
         <v>76</v>
       </c>
       <c r="I5" s="43">
-        <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122</f>
-        <v>11030000</v>
+        <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122+E135</f>
+        <v>11350000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2115,6 +2124,115 @@
         <v>35</v>
       </c>
     </row>
+    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127" s="36"/>
+      <c r="B127" s="36"/>
+      <c r="C127" s="36"/>
+      <c r="D127" s="36"/>
+      <c r="E127" s="36"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B129" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C129" s="2"/>
+      <c r="E129" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B130" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C130" s="2">
+        <v>2</v>
+      </c>
+      <c r="E130" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B131" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C131" s="2">
+        <v>2</v>
+      </c>
+      <c r="E131" s="11"/>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B132" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C132" s="2">
+        <v>4</v>
+      </c>
+      <c r="E132" s="11"/>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B133" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C133" s="2"/>
+      <c r="E133" s="11"/>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B134" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C134" s="2"/>
+    </row>
+    <row r="135" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B135" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C135" s="2"/>
+      <c r="E135" s="42">
+        <f>C136*40000</f>
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B136" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" s="19">
+        <f>SUM(C129:C135)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C137" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D137" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C138" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D138" s="21">
+        <f>C136-D137</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
complete and working registration process
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>Hours</t>
   </si>
@@ -282,7 +282,10 @@
     <t>• Fix tracker's crash</t>
   </si>
   <si>
-    <t>• Added tracker status messages</t>
+    <t>• Added tracker status splash messages</t>
+  </si>
+  <si>
+    <t>• Complete and working registration process</t>
   </si>
 </sst>
 </file>
@@ -904,7 +907,7 @@
   <dimension ref="A2:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,7 +974,7 @@
       </c>
       <c r="I5" s="43">
         <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122+E135</f>
-        <v>11350000</v>
+        <v>11430000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2171,9 +2174,11 @@
         <v>43</v>
       </c>
       <c r="C131" s="2">
-        <v>2</v>
-      </c>
-      <c r="E131" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="E131" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
@@ -2204,7 +2209,7 @@
       <c r="C135" s="2"/>
       <c r="E135" s="42">
         <f>C136*40000</f>
-        <v>320000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.3">
@@ -2213,7 +2218,7 @@
       </c>
       <c r="C136" s="19">
         <f>SUM(C129:C135)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.3">
@@ -2230,7 +2235,7 @@
       </c>
       <c r="D138" s="21">
         <f>C136-D137</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
release 2020-11 phantom version
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -279,13 +279,13 @@
     <t>آذر 99</t>
   </si>
   <si>
-    <t>• Fix tracker's crash</t>
-  </si>
-  <si>
     <t>• Added tracker status splash messages</t>
   </si>
   <si>
     <t>• Complete and working registration process</t>
+  </si>
+  <si>
+    <t>• Fixed tracker's crash</t>
   </si>
 </sst>
 </file>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="C129" s="2"/>
       <c r="E129" s="39" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.3">
@@ -2166,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.3">
@@ -2177,7 +2177,7 @@
         <v>4</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Show dual view of points before registration
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -907,7 +907,7 @@
   <dimension ref="A2:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,7 +974,7 @@
       </c>
       <c r="I5" s="43">
         <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122+E135</f>
-        <v>11430000</v>
+        <v>11510000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2206,10 +2206,12 @@
       <c r="B135" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C135" s="2"/>
+      <c r="C135" s="2">
+        <v>2</v>
+      </c>
       <c r="E135" s="42">
         <f>C136*40000</f>
-        <v>400000</v>
+        <v>480000</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.3">
@@ -2218,7 +2220,7 @@
       </c>
       <c r="C136" s="19">
         <f>SUM(C129:C135)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.3">
@@ -2235,7 +2237,7 @@
       </c>
       <c r="D138" s="21">
         <f>C136-D137</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed errors in new/load/delete patients
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
   <si>
     <t>Hours</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>• Fixed tracker's crash</t>
+  </si>
+  <si>
+    <t>* Patients / Database</t>
   </si>
 </sst>
 </file>
@@ -906,25 +909,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.88671875" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.90625" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.90625" customWidth="1"/>
     <col min="12" max="12" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
@@ -933,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="27" t="s">
         <v>15</v>
       </c>
@@ -946,7 +949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="H4" s="40" t="s">
         <v>4</v>
       </c>
@@ -955,7 +958,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
@@ -974,10 +977,10 @@
       </c>
       <c r="I5" s="43">
         <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122+E135</f>
-        <v>11510000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11630000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
@@ -989,7 +992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1010,7 +1013,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1019,7 +1022,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +1031,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>1020000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="12" t="s">
         <v>2</v>
@@ -1051,7 +1054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" s="12" t="s">
         <v>3</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1068,7 +1071,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1124,7 +1127,7 @@
       </c>
       <c r="E20" s="37"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="33" t="s">
         <v>4</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>1350000</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C23" s="4" t="s">
         <v>2</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C24" s="4" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1170,7 +1173,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="32" t="s">
         <v>14</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28" s="31" t="s">
         <v>23</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" s="28" t="s">
         <v>26</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>12</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B34" s="33" t="s">
         <v>4</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>1020000</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C35" s="4" t="s">
         <v>2</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C36" s="4" t="s">
         <v>3</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1279,7 +1282,7 @@
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
         <v>27</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B40" s="28" t="s">
         <v>26</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>39</v>
       </c>
@@ -1335,7 +1338,7 @@
       </c>
       <c r="E43" s="35"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>40</v>
       </c>
@@ -1344,7 +1347,7 @@
       </c>
       <c r="E44" s="35"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B45" s="33" t="s">
         <v>4</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C47" s="4" t="s">
         <v>3</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -1382,14 +1385,14 @@
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="36"/>
       <c r="B49" s="36"/>
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
       <c r="E49" s="36"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="32" t="s">
         <v>32</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>16</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>39</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>36</v>
       </c>
@@ -1447,7 +1450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
         <v>41</v>
       </c>
@@ -1456,7 +1459,7 @@
       </c>
       <c r="E55" s="35"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
         <v>35</v>
       </c>
@@ -1465,7 +1468,7 @@
       </c>
       <c r="E56" s="35"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B57" s="33" t="s">
         <v>4</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C58" s="4" t="s">
         <v>2</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C59" s="4" t="s">
         <v>3</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -1503,14 +1506,14 @@
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="36"/>
       <c r="B61" s="36"/>
       <c r="C61" s="36"/>
       <c r="D61" s="36"/>
       <c r="E61" s="36"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="32" t="s">
         <v>48</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B63" s="1" t="s">
         <v>17</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B64" s="1" t="s">
         <v>47</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B65" s="1" t="s">
         <v>42</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B66" s="1" t="s">
         <v>45</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B67" s="1" t="s">
         <v>49</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B68" s="1" t="s">
         <v>43</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B69" s="1" t="s">
         <v>46</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B70" s="1" t="s">
         <v>44</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B71" s="1" t="s">
         <v>13</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B72" s="33" t="s">
         <v>4</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C73" s="4" t="s">
         <v>2</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C74" s="4" t="s">
         <v>3</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -1646,14 +1649,14 @@
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="36"/>
       <c r="B76" s="36"/>
       <c r="C76" s="36"/>
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="32" t="s">
         <v>50</v>
       </c>
@@ -1667,7 +1670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B78" s="1" t="s">
         <v>51</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B79" s="1" t="s">
         <v>52</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
         <v>53</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
         <v>47</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B82" s="1" t="s">
         <v>54</v>
       </c>
@@ -1716,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B83" s="33" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>680000</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C84" s="4" t="s">
         <v>2</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C85" s="4" t="s">
         <v>3</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -1754,14 +1757,14 @@
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="36"/>
       <c r="B87" s="36"/>
       <c r="C87" s="36"/>
       <c r="D87" s="36"/>
       <c r="E87" s="36"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="32" t="s">
         <v>71</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B89" s="1" t="s">
         <v>53</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B90" s="1" t="s">
         <v>65</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B91" s="1" t="s">
         <v>46</v>
       </c>
@@ -1808,7 +1811,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B92" s="1" t="s">
         <v>43</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B93" s="1" t="s">
         <v>56</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B94" s="1" t="s">
         <v>47</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B95" s="1" t="s">
         <v>66</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B96" s="1" t="s">
         <v>67</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B97" s="1" t="s">
         <v>55</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B98" s="33" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1875,7 @@
         <v>1360000</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C99" s="4" t="s">
         <v>2</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C100" s="4" t="s">
         <v>3</v>
       </c>
@@ -1889,7 +1892,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="14"/>
       <c r="B102" s="14"/>
       <c r="C102" s="14"/>
@@ -1898,14 +1901,14 @@
       <c r="F102" s="14"/>
       <c r="G102" s="14"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="36"/>
       <c r="B103" s="36"/>
       <c r="C103" s="36"/>
       <c r="D103" s="36"/>
       <c r="E103" s="36"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="32" t="s">
         <v>72</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B105" s="1" t="s">
         <v>74</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B106" s="1" t="s">
         <v>47</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B107" s="1" t="s">
         <v>43</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B108" s="1" t="s">
         <v>78</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B109" s="1" t="s">
         <v>77</v>
       </c>
@@ -1966,7 +1969,7 @@
       </c>
       <c r="E109" s="35"/>
     </row>
-    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B110" s="33" t="s">
         <v>4</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C111" s="4" t="s">
         <v>2</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C112" s="4" t="s">
         <v>3</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="14"/>
       <c r="B113" s="14"/>
       <c r="C113" s="14"/>
@@ -2005,14 +2008,14 @@
       <c r="F113" s="14"/>
       <c r="G113" s="14"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="36"/>
       <c r="B114" s="36"/>
       <c r="C114" s="36"/>
       <c r="D114" s="36"/>
       <c r="E114" s="36"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="25" t="s">
         <v>80</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B116" s="1" t="s">
         <v>52</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B117" s="1" t="s">
         <v>47</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B118" s="1" t="s">
         <v>43</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B119" s="1" t="s">
         <v>78</v>
       </c>
@@ -2070,7 +2073,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B120" s="1" t="s">
         <v>45</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B121" s="1" t="s">
         <v>74</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B122" s="1" t="s">
         <v>77</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B123" s="18" t="s">
         <v>4</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C124" s="4" t="s">
         <v>2</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C125" s="4" t="s">
         <v>3</v>
       </c>
@@ -2127,15 +2130,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="36"/>
       <c r="B127" s="36"/>
       <c r="C127" s="36"/>
       <c r="D127" s="36"/>
       <c r="E127" s="36"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="25" t="s">
         <v>85</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B129" s="1" t="s">
         <v>52</v>
       </c>
@@ -2158,18 +2161,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B130" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C130" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E130" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B131" s="1" t="s">
         <v>43</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B132" s="1" t="s">
         <v>78</v>
       </c>
@@ -2189,20 +2192,22 @@
       </c>
       <c r="E132" s="11"/>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B133" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C133" s="2"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B134" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C134" s="2"/>
-    </row>
-    <row r="135" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="C134" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B135" s="1" t="s">
         <v>77</v>
       </c>
@@ -2211,19 +2216,19 @@
       </c>
       <c r="E135" s="42">
         <f>C136*40000</f>
-        <v>480000</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B136" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C136" s="19">
         <f>SUM(C129:C135)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C137" s="4" t="s">
         <v>2</v>
       </c>
@@ -2231,13 +2236,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C138" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D138" s="21">
         <f>C136-D137</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last master before multilayout
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -910,24 +910,24 @@
   <dimension ref="A2:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.90625" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.88671875" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
     <col min="12" max="12" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
@@ -936,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>15</v>
       </c>
@@ -949,7 +949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H4" s="40" t="s">
         <v>4</v>
       </c>
@@ -958,7 +958,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
@@ -977,10 +977,10 @@
       </c>
       <c r="I5" s="43">
         <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122+E135</f>
-        <v>11630000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>11750000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
@@ -992,7 +992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>1020000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
       <c r="C12" s="12" t="s">
         <v>2</v>
@@ -1054,7 +1054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" s="12" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1071,7 +1071,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="E20" s="37"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="33" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>1350000</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C24" s="4" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1173,7 +1173,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="32" t="s">
         <v>14</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="31" t="s">
         <v>23</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="28" t="s">
         <v>26</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="33" t="s">
         <v>4</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>1020000</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C35" s="4" t="s">
         <v>2</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C36" s="4" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1282,7 +1282,7 @@
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="32" t="s">
         <v>27</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B40" s="28" t="s">
         <v>26</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>39</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="E43" s="35"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>40</v>
       </c>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="E44" s="35"/>
     </row>
-    <row r="45" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="33" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C46" s="4" t="s">
         <v>2</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C47" s="4" t="s">
         <v>3</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -1385,14 +1385,14 @@
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="36"/>
       <c r="B49" s="36"/>
       <c r="C49" s="36"/>
       <c r="D49" s="36"/>
       <c r="E49" s="36"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="32" t="s">
         <v>32</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>16</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>39</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>36</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>41</v>
       </c>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="E55" s="35"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>35</v>
       </c>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="E56" s="35"/>
     </row>
-    <row r="57" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B57" s="33" t="s">
         <v>4</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C58" s="4" t="s">
         <v>2</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C59" s="4" t="s">
         <v>3</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -1506,14 +1506,14 @@
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="36"/>
       <c r="B61" s="36"/>
       <c r="C61" s="36"/>
       <c r="D61" s="36"/>
       <c r="E61" s="36"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="32" t="s">
         <v>48</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>17</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>47</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>42</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="s">
         <v>45</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>49</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
         <v>43</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>46</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
         <v>44</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B72" s="33" t="s">
         <v>4</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C73" s="4" t="s">
         <v>2</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C74" s="4" t="s">
         <v>3</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -1649,14 +1649,14 @@
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="36"/>
       <c r="B76" s="36"/>
       <c r="C76" s="36"/>
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="32" t="s">
         <v>50</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>51</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
         <v>52</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>53</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
         <v>47</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>54</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B83" s="33" t="s">
         <v>4</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>680000</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C84" s="4" t="s">
         <v>2</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C85" s="4" t="s">
         <v>3</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -1757,14 +1757,14 @@
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="36"/>
       <c r="B87" s="36"/>
       <c r="C87" s="36"/>
       <c r="D87" s="36"/>
       <c r="E87" s="36"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="32" t="s">
         <v>71</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>53</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
         <v>65</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
         <v>46</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B92" s="1" t="s">
         <v>43</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
         <v>56</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
         <v>47</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
         <v>66</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
         <v>67</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
         <v>55</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B98" s="33" t="s">
         <v>4</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>1360000</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C99" s="4" t="s">
         <v>2</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C100" s="4" t="s">
         <v>3</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="14"/>
       <c r="B102" s="14"/>
       <c r="C102" s="14"/>
@@ -1901,14 +1901,14 @@
       <c r="F102" s="14"/>
       <c r="G102" s="14"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="36"/>
       <c r="B103" s="36"/>
       <c r="C103" s="36"/>
       <c r="D103" s="36"/>
       <c r="E103" s="36"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="32" t="s">
         <v>72</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
         <v>74</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
         <v>47</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
         <v>43</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
         <v>78</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
         <v>77</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="E109" s="35"/>
     </row>
-    <row r="110" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B110" s="33" t="s">
         <v>4</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C111" s="4" t="s">
         <v>2</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C112" s="4" t="s">
         <v>3</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="14"/>
       <c r="B113" s="14"/>
       <c r="C113" s="14"/>
@@ -2008,14 +2008,14 @@
       <c r="F113" s="14"/>
       <c r="G113" s="14"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="36"/>
       <c r="B114" s="36"/>
       <c r="C114" s="36"/>
       <c r="D114" s="36"/>
       <c r="E114" s="36"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
         <v>80</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B116" s="1" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B117" s="1" t="s">
         <v>47</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B118" s="1" t="s">
         <v>43</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
         <v>78</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
         <v>45</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
         <v>74</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>77</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B123" s="18" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C124" s="4" t="s">
         <v>2</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C125" s="4" t="s">
         <v>3</v>
       </c>
@@ -2130,15 +2130,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="36"/>
       <c r="B127" s="36"/>
       <c r="C127" s="36"/>
       <c r="D127" s="36"/>
       <c r="E127" s="36"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="25" t="s">
         <v>85</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B129" s="1" t="s">
         <v>52</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B130" s="1" t="s">
         <v>47</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
         <v>43</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>78</v>
       </c>
@@ -2192,14 +2192,14 @@
       </c>
       <c r="E132" s="11"/>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C133" s="2"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>89</v>
       </c>
@@ -2207,28 +2207,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C135" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E135" s="42">
         <f>C136*40000</f>
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.35">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B136" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C136" s="19">
         <f>SUM(C129:C135)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C137" s="4" t="s">
         <v>2</v>
       </c>
@@ -2236,13 +2236,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C138" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D138" s="21">
         <f>C136-D137</f>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bigger points in 3D views & minor bug fixes
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
   <si>
     <t>Hours</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>• Document of the code</t>
+  </si>
+  <si>
+    <t>دی 99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• </t>
   </si>
 </sst>
 </file>
@@ -919,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I138"/>
+  <dimension ref="A2:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2164,7 +2170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B129" s="1" t="s">
         <v>92</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B130" s="1" t="s">
         <v>47</v>
       </c>
@@ -2186,7 +2192,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
         <v>43</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>78</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>45</v>
       </c>
@@ -2219,7 +2225,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>89</v>
       </c>
@@ -2227,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>90</v>
       </c>
@@ -2239,7 +2245,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B136" s="18" t="s">
         <v>4</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C137" s="4" t="s">
         <v>2</v>
       </c>
@@ -2256,13 +2262,124 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C138" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D138" s="21">
         <f>C136-D137</f>
         <v>29</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" s="36"/>
+      <c r="B140" s="36"/>
+      <c r="C140" s="36"/>
+      <c r="D140" s="36"/>
+      <c r="E140" s="36"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E141" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B142" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C142" s="2"/>
+      <c r="E142" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B143" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C143" s="2"/>
+      <c r="E143" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B144" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C144" s="2"/>
+      <c r="E144" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B145" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C145" s="2"/>
+      <c r="E145" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B146" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C146" s="2"/>
+      <c r="E146" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B147" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C147" s="2"/>
+    </row>
+    <row r="148" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B148" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C148" s="2">
+        <v>1</v>
+      </c>
+      <c r="E148" s="42">
+        <f>C149*40000</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B149" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" s="19">
+        <f>SUM(C142:C148)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C150" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D150" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C151" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D151" s="21">
+        <f>C149-D150</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added moving light to 3D camera in virtual mode
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="97">
   <si>
     <t>Hours</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t xml:space="preserve">• </t>
+  </si>
+  <si>
+    <t>* Segmentation</t>
   </si>
 </sst>
 </file>
@@ -927,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,8 +997,8 @@
         <v>76</v>
       </c>
       <c r="I5" s="43">
-        <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122+E135</f>
-        <v>12430000</v>
+        <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122</f>
+        <v>11030000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2034,7 +2037,7 @@
       <c r="E114" s="36"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A115" s="25" t="s">
+      <c r="A115" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B115" s="7" t="s">
@@ -2123,10 +2126,10 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B123" s="18" t="s">
+      <c r="B123" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="19">
+      <c r="C123" s="34">
         <f>SUM(C116:C122)</f>
         <v>35</v>
       </c>
@@ -2148,7 +2151,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+    </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="36"/>
       <c r="B127" s="36"/>
@@ -2170,7 +2176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B129" s="1" t="s">
         <v>92</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B130" s="1" t="s">
         <v>47</v>
       </c>
@@ -2192,7 +2198,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
         <v>43</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>78</v>
       </c>
@@ -2214,7 +2220,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>45</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>89</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>90</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B136" s="18" t="s">
         <v>4</v>
       </c>
@@ -2254,7 +2260,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C137" s="4" t="s">
         <v>2</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C138" s="4" t="s">
         <v>3</v>
       </c>
@@ -2271,15 +2277,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="36"/>
       <c r="B140" s="36"/>
       <c r="C140" s="36"/>
       <c r="D140" s="36"/>
       <c r="E140" s="36"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="25" t="s">
         <v>94</v>
       </c>
@@ -2293,16 +2302,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B142" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C142" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="C142" s="2">
+        <v>2</v>
+      </c>
       <c r="E142" s="39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
         <v>47</v>
       </c>
@@ -2311,11 +2322,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B144" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C144" s="2"/>
+      <c r="C144" s="2">
+        <v>2</v>
+      </c>
       <c r="E144" s="11" t="s">
         <v>95</v>
       </c>
@@ -2324,7 +2337,9 @@
       <c r="B145" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C145" s="2"/>
+      <c r="C145" s="2">
+        <v>1</v>
+      </c>
       <c r="E145" s="11" t="s">
         <v>95</v>
       </c>
@@ -2349,11 +2364,11 @@
         <v>90</v>
       </c>
       <c r="C148" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E148" s="42">
         <f>C149*40000</f>
-        <v>40000</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.3">
@@ -2362,7 +2377,7 @@
       </c>
       <c r="C149" s="19">
         <f>SUM(C142:C148)</f>
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.3">
@@ -2370,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="D150" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.3">
@@ -2379,7 +2394,7 @@
       </c>
       <c r="D151" s="21">
         <f>C149-D150</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for new patient crash + main window size change on load image
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
   <si>
     <t>Hours</t>
   </si>
@@ -310,6 +310,18 @@
   </si>
   <si>
     <t>* Segmentation</t>
+  </si>
+  <si>
+    <t>• More realistic virtual view</t>
+  </si>
+  <si>
+    <t>@IACT</t>
+  </si>
+  <si>
+    <t>* Debug &amp; Refactor</t>
+  </si>
+  <si>
+    <t>• Bug and Crash Fixes</t>
   </si>
 </sst>
 </file>
@@ -928,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I151"/>
+  <dimension ref="A2:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2262,7 +2274,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C137" s="4" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="D137" s="3">
         <v>6</v>
@@ -2315,11 +2327,13 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C143" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C143" s="2">
+        <v>1</v>
+      </c>
       <c r="E143" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -2338,63 +2352,56 @@
         <v>78</v>
       </c>
       <c r="C145" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E145" s="11" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B146" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C146" s="2"/>
-      <c r="E146" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C146" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B147" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C147" s="2"/>
-    </row>
-    <row r="148" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B148" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C148" s="2">
-        <v>10</v>
-      </c>
-      <c r="E148" s="42">
-        <f>C149*40000</f>
-        <v>600000</v>
+      <c r="C147" s="2">
+        <v>28</v>
+      </c>
+      <c r="E147" s="42">
+        <f>C148*40000</f>
+        <v>1640000</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B148" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C148" s="19">
+        <f>SUM(C142:C147)</f>
+        <v>41</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B149" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C149" s="19">
-        <f>SUM(C142:C148)</f>
-        <v>15</v>
+      <c r="C149" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D149" s="3">
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C150" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D150" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C151" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D151" s="21">
-        <f>C149-D150</f>
-        <v>4</v>
+      <c r="D150" s="21">
+        <f>C148-D149</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new layout with three 2d views
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="105">
   <si>
     <t>Hours</t>
   </si>
@@ -306,9 +306,6 @@
     <t>دی 99</t>
   </si>
   <si>
-    <t xml:space="preserve">• </t>
-  </si>
-  <si>
     <t>* Segmentation</t>
   </si>
   <si>
@@ -322,6 +319,21 @@
   </si>
   <si>
     <t>• Bug and Crash Fixes</t>
+  </si>
+  <si>
+    <t>* BronchoVision Video</t>
+  </si>
+  <si>
+    <t>• BronchoVision Video</t>
+  </si>
+  <si>
+    <t>* Presentations</t>
+  </si>
+  <si>
+    <t>* Camera preparation</t>
+  </si>
+  <si>
+    <t>بهمن و اسفند 99</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,12 +460,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,21 +622,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -648,16 +651,19 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="12" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -940,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I150"/>
+  <dimension ref="A2:I162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I159" sqref="I159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,7 +967,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="17"/>
@@ -970,7 +976,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="14"/>
@@ -983,16 +989,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="41">
+      <c r="I4" s="40">
         <f>C11+C22+C34+C45+C57+C72+C83+C98+C110+C123</f>
         <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1005,12 +1011,12 @@
       <c r="E5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="43">
-        <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122</f>
-        <v>11030000</v>
+      <c r="I5" s="42">
+        <f>E11+E22+E34+E45+E57+E72+E83+E98+E110+E122+E135+E147</f>
+        <v>14230000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1073,7 +1079,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="42">
+      <c r="E11" s="41">
         <f>C11*30000</f>
         <v>1020000</v>
       </c>
@@ -1105,7 +1111,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1158,7 +1164,7 @@
       <c r="C20" s="2">
         <v>4</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="36"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
@@ -1169,14 +1175,14 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="33">
         <f>SUM(C17:C21)</f>
         <v>45</v>
       </c>
-      <c r="E22" s="42">
+      <c r="E22" s="41">
         <f>C22*30000</f>
         <v>1350000</v>
       </c>
@@ -1207,7 +1213,7 @@
       <c r="G25" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -1221,10 +1227,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="29">
         <v>10</v>
       </c>
       <c r="E28" s="11" t="s">
@@ -1232,10 +1238,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="29">
+      <c r="C29" s="28">
         <v>15</v>
       </c>
       <c r="E29" s="11" t="s">
@@ -1278,14 +1284,14 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="33">
         <f>SUM(C28:C33)</f>
         <v>34</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="41">
         <f>C34*30000</f>
         <v>1020000</v>
       </c>
@@ -1316,7 +1322,7 @@
       <c r="G37" s="14"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1330,10 +1336,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="29">
+      <c r="C40" s="28">
         <v>3</v>
       </c>
       <c r="E40" s="11" t="s">
@@ -1369,7 +1375,7 @@
       <c r="C43" s="2">
         <v>4</v>
       </c>
-      <c r="E43" s="35"/>
+      <c r="E43" s="34"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
@@ -1378,17 +1384,17 @@
       <c r="C44" s="2">
         <v>7</v>
       </c>
-      <c r="E44" s="35"/>
+      <c r="E44" s="34"/>
     </row>
     <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="34">
+      <c r="C45" s="33">
         <f>SUM(C40:C44)</f>
         <v>20</v>
       </c>
-      <c r="E45" s="42">
+      <c r="E45" s="41">
         <f>C45*30000</f>
         <v>600000</v>
       </c>
@@ -1419,14 +1425,14 @@
       <c r="G48" s="14"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="31" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="7" t="s">
@@ -1490,7 +1496,7 @@
       <c r="C55" s="2">
         <v>4</v>
       </c>
-      <c r="E55" s="35"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
@@ -1499,17 +1505,17 @@
       <c r="C56" s="2">
         <v>1</v>
       </c>
-      <c r="E56" s="35"/>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="34">
+      <c r="C57" s="33">
         <f>SUM(C51:C56)</f>
         <v>40</v>
       </c>
-      <c r="E57" s="42">
+      <c r="E57" s="41">
         <f>C57*30000</f>
         <v>1200000</v>
       </c>
@@ -1540,14 +1546,14 @@
       <c r="G60" s="14"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
+      <c r="A61" s="35"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="32" t="s">
+      <c r="A62" s="31" t="s">
         <v>48</v>
       </c>
       <c r="B62" s="7" t="s">
@@ -1567,7 +1573,7 @@
       <c r="C63" s="2">
         <v>5</v>
       </c>
-      <c r="E63" s="39" t="s">
+      <c r="E63" s="38" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1645,14 +1651,14 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="34">
+      <c r="C72" s="33">
         <f>SUM(C63:C71)</f>
         <v>40</v>
       </c>
-      <c r="E72" s="42">
+      <c r="E72" s="41">
         <f>C72*20000</f>
         <v>800000</v>
       </c>
@@ -1683,14 +1689,14 @@
       <c r="G75" s="14"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="36"/>
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
+      <c r="A76" s="35"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="32" t="s">
+      <c r="A77" s="31" t="s">
         <v>50</v>
       </c>
       <c r="B77" s="7" t="s">
@@ -1710,7 +1716,7 @@
       <c r="C78" s="2">
         <v>1</v>
       </c>
-      <c r="E78" s="39" t="s">
+      <c r="E78" s="38" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1753,14 +1759,14 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B83" s="33" t="s">
+      <c r="B83" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="34">
+      <c r="C83" s="33">
         <f>SUM(C78:C82)</f>
         <v>17</v>
       </c>
-      <c r="E83" s="42">
+      <c r="E83" s="41">
         <f>C83*40000</f>
         <v>680000</v>
       </c>
@@ -1791,14 +1797,14 @@
       <c r="G86" s="14"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="36"/>
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
+      <c r="A87" s="35"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="35"/>
+      <c r="D87" s="35"/>
+      <c r="E87" s="35"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="32" t="s">
+      <c r="A88" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -1818,7 +1824,7 @@
       <c r="C89" s="2">
         <v>1</v>
       </c>
-      <c r="E89" s="39" t="s">
+      <c r="E89" s="38" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1896,14 +1902,14 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B98" s="33" t="s">
+      <c r="B98" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C98" s="34">
+      <c r="C98" s="33">
         <f>SUM(C89:C97)</f>
         <v>34</v>
       </c>
-      <c r="E98" s="42">
+      <c r="E98" s="41">
         <f>C98*40000</f>
         <v>1360000</v>
       </c>
@@ -1935,14 +1941,14 @@
       <c r="G102" s="14"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="36"/>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="32" t="s">
+      <c r="A104" s="31" t="s">
         <v>72</v>
       </c>
       <c r="B104" s="7" t="s">
@@ -1962,7 +1968,7 @@
       <c r="C105" s="2">
         <v>9</v>
       </c>
-      <c r="E105" s="39" t="s">
+      <c r="E105" s="38" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2000,17 +2006,17 @@
       <c r="C109" s="2">
         <v>5</v>
       </c>
-      <c r="E109" s="35"/>
+      <c r="E109" s="34"/>
     </row>
     <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B110" s="33" t="s">
+      <c r="B110" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C110" s="34">
+      <c r="C110" s="33">
         <f>SUM(C105:C109)</f>
         <v>40</v>
       </c>
-      <c r="E110" s="42">
+      <c r="E110" s="41">
         <f>C110*40000</f>
         <v>1600000</v>
       </c>
@@ -2042,14 +2048,14 @@
       <c r="G113" s="14"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A114" s="36"/>
-      <c r="B114" s="36"/>
-      <c r="C114" s="36"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
+      <c r="A114" s="35"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
+      <c r="E114" s="35"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A115" s="32" t="s">
+      <c r="A115" s="31" t="s">
         <v>80</v>
       </c>
       <c r="B115" s="7" t="s">
@@ -2069,7 +2075,7 @@
       <c r="C116" s="2">
         <v>6</v>
       </c>
-      <c r="E116" s="39" t="s">
+      <c r="E116" s="38" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2132,16 +2138,16 @@
       <c r="C122" s="2">
         <v>2</v>
       </c>
-      <c r="E122" s="42">
+      <c r="E122" s="41">
         <f>C123*40000</f>
         <v>1400000</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B123" s="33" t="s">
+      <c r="B123" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="34">
+      <c r="C123" s="33">
         <f>SUM(C116:C122)</f>
         <v>35</v>
       </c>
@@ -2168,14 +2174,14 @@
       <c r="G126" s="14"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="36"/>
-      <c r="B127" s="36"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="36"/>
-      <c r="E127" s="36"/>
+      <c r="A127" s="35"/>
+      <c r="B127" s="35"/>
+      <c r="C127" s="35"/>
+      <c r="D127" s="35"/>
+      <c r="E127" s="35"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A128" s="25" t="s">
+      <c r="A128" s="31" t="s">
         <v>85</v>
       </c>
       <c r="B128" s="7" t="s">
@@ -2195,7 +2201,7 @@
       <c r="C129" s="2">
         <v>3</v>
       </c>
-      <c r="E129" s="39" t="s">
+      <c r="E129" s="38" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2258,23 +2264,23 @@
       <c r="C135" s="2">
         <v>12</v>
       </c>
-      <c r="E135" s="42">
+      <c r="E135" s="41">
         <f>C136*40000</f>
         <v>1400000</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B136" s="18" t="s">
+      <c r="B136" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C136" s="19">
+      <c r="C136" s="33">
         <f>SUM(C129:C135)</f>
         <v>35</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C137" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D137" s="3">
         <v>6</v>
@@ -2294,14 +2300,14 @@
       <c r="G139" s="14"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A140" s="36"/>
-      <c r="B140" s="36"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="36"/>
-      <c r="E140" s="36"/>
+      <c r="A140" s="35"/>
+      <c r="B140" s="35"/>
+      <c r="C140" s="35"/>
+      <c r="D140" s="35"/>
+      <c r="E140" s="35"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A141" s="25" t="s">
+      <c r="A141" s="31" t="s">
         <v>94</v>
       </c>
       <c r="B141" s="7" t="s">
@@ -2316,24 +2322,24 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B142" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C142" s="2">
         <v>2</v>
       </c>
-      <c r="E142" s="39" t="s">
+      <c r="E142" s="38" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C143" s="2">
         <v>1</v>
       </c>
       <c r="E143" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -2344,10 +2350,10 @@
         <v>2</v>
       </c>
       <c r="E144" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B145" s="1" t="s">
         <v>78</v>
       </c>
@@ -2355,10 +2361,10 @@
         <v>5</v>
       </c>
       <c r="E145" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B146" s="1" t="s">
         <v>45</v>
       </c>
@@ -2366,42 +2372,145 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B147" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C147" s="2">
+        <v>4</v>
+      </c>
+      <c r="E147" s="41">
+        <f>C149*40000</f>
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B148" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C147" s="2">
+      <c r="C148" s="2">
         <v>28</v>
       </c>
-      <c r="E147" s="42">
-        <f>C148*40000</f>
-        <v>1640000</v>
-      </c>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B148" s="18" t="s">
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B149" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C148" s="19">
-        <f>SUM(C142:C147)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C149" s="4" t="s">
+      <c r="C149" s="33">
+        <f>SUM(C142:C148)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C150" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D150" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C151" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D151" s="21">
+        <f>C149-D150</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F152" s="14"/>
+      <c r="G152" s="14"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A153" s="35"/>
+      <c r="B153" s="35"/>
+      <c r="C153" s="35"/>
+      <c r="D153" s="35"/>
+      <c r="E153" s="35"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E154" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B155" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C155" s="2">
+        <v>1</v>
+      </c>
+      <c r="E155" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B156" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D149" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C150" s="4" t="s">
+      <c r="C156" s="2"/>
+      <c r="E156" s="11"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B157" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C157" s="2"/>
+      <c r="E157" s="11"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B158" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C158" s="2"/>
+      <c r="E158" s="11"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B159" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C159" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B160" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C160" s="19">
+        <f>SUM(C155:C159)</f>
+        <v>9</v>
+      </c>
+      <c r="E160" s="41">
+        <f>C160*40000</f>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="161" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C161" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D161" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C162" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D150" s="21">
-        <f>C148-D149</f>
-        <v>9</v>
+      <c r="D162" s="21">
+        <f>C160-D161</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
list available cameras + better window size handling
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="107">
   <si>
     <t>Hours</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>بهمن و اسفند 99</t>
+  </si>
+  <si>
+    <t>* Video Camera</t>
+  </si>
+  <si>
+    <t>• Integrated Video Camera</t>
   </si>
 </sst>
 </file>
@@ -949,7 +955,7 @@
   <dimension ref="A2:I162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="I159" sqref="I159"/>
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2459,20 +2465,26 @@
         <v>98</v>
       </c>
       <c r="C156" s="2"/>
-      <c r="E156" s="11"/>
+      <c r="E156" s="11" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B157" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C157" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="C157" s="2">
+        <v>4</v>
+      </c>
       <c r="E157" s="11"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B158" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C158" s="2"/>
+      <c r="C158" s="2">
+        <v>1</v>
+      </c>
       <c r="E158" s="11"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -2489,11 +2501,11 @@
       </c>
       <c r="C160" s="19">
         <f>SUM(C155:C159)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E160" s="41">
         <f>C160*40000</f>
-        <v>360000</v>
+        <v>560000</v>
       </c>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.3">
@@ -2510,7 +2522,7 @@
       </c>
       <c r="D162" s="21">
         <f>C160-D161</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last status from 20201-03
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B503119E-C077-4914-945F-356E13FB7312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="117">
   <si>
     <t>Hours</t>
   </si>
@@ -340,12 +348,42 @@
   </si>
   <si>
     <t>• Integrated Video Camera</t>
+  </si>
+  <si>
+    <t>بهار 1400</t>
+  </si>
+  <si>
+    <t>* Debugging</t>
+  </si>
+  <si>
+    <t>* System Preparation</t>
+  </si>
+  <si>
+    <t>• Meeting with chinese team @Parsiss</t>
+  </si>
+  <si>
+    <t>• Navigation with Video Camera</t>
+  </si>
+  <si>
+    <t>* Data Preparation</t>
+  </si>
+  <si>
+    <t>• Deep Segmentation Model</t>
+  </si>
+  <si>
+    <t>* Deep Model Code</t>
+  </si>
+  <si>
+    <t>• Lung/Airway Segmentation Data</t>
+  </si>
+  <si>
+    <t>پاییز 1400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,11 +989,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I162"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C158" sqref="C158"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J174" sqref="J174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2436,7 +2474,7 @@
       <c r="E153" s="35"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A154" s="43" t="s">
+      <c r="A154" s="31" t="s">
         <v>104</v>
       </c>
       <c r="B154" s="7" t="s">
@@ -2462,67 +2500,238 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B156" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C156" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="C156" s="2">
+        <v>4</v>
+      </c>
       <c r="E156" s="11" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B157" s="1" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C157" s="2">
-        <v>4</v>
-      </c>
-      <c r="E157" s="11"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B158" s="1" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="C158" s="2">
+        <v>8</v>
+      </c>
+      <c r="E158" s="41">
+        <f>C159*40000</f>
+        <v>560000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B159" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C159" s="33">
+        <f>SUM(C155:C158)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C160" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D160" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C161" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D161" s="21">
+        <f>C159-D160</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F162" s="14"/>
+      <c r="G162" s="14"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A163" s="35"/>
+      <c r="B163" s="35"/>
+      <c r="C163" s="35"/>
+      <c r="D163" s="35"/>
+      <c r="E163" s="35"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A164" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C164" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E164" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B165" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C165" s="2">
+        <v>4</v>
+      </c>
+      <c r="E165" s="38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B166" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C166" s="2">
+        <v>3</v>
+      </c>
+      <c r="E166" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B167" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C167" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B168" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C168" s="19">
+        <f>SUM(C165:C167)</f>
+        <v>10</v>
+      </c>
+      <c r="E168" s="41">
+        <f>C168*40000</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C169" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D169" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C170" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D170" s="21">
+        <f>C168-D169</f>
         <v>1</v>
       </c>
-      <c r="E158" s="11"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B159" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C159" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B160" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C160" s="19">
-        <f>SUM(C155:C159)</f>
-        <v>14</v>
-      </c>
-      <c r="E160" s="41">
-        <f>C160*40000</f>
-        <v>560000</v>
-      </c>
-    </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C161" s="4" t="s">
+    </row>
+    <row r="171" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F171" s="14"/>
+      <c r="G171" s="14"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A172" s="35"/>
+      <c r="B172" s="35"/>
+      <c r="C172" s="35"/>
+      <c r="D172" s="35"/>
+      <c r="E172" s="35"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A173" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E173" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B174" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C174" s="2">
+        <v>5</v>
+      </c>
+      <c r="E174" s="38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B175" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C175" s="2">
+        <v>5</v>
+      </c>
+      <c r="E175" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B176" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C176" s="2">
+        <v>6</v>
+      </c>
+      <c r="E176" s="34"/>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B177" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C177" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B178" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178" s="19">
+        <f>SUM(C174:C177)</f>
+        <v>19</v>
+      </c>
+      <c r="E178" s="41">
+        <f>C178*40000</f>
+        <v>760000</v>
+      </c>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C179" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D161" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C162" s="4" t="s">
+      <c r="D179" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C180" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D162" s="21">
-        <f>C160-D161</f>
-        <v>7</v>
+      <c r="D180" s="21">
+        <f>C178-D179</f>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated environment.yml, README, TimeSheet
</commit_message>
<xml_diff>
--- a/other/TimeSheet.xlsx
+++ b/other/TimeSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B503119E-C077-4914-945F-356E13FB7312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A714D7-219B-40F0-9404-752E7466F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J174" sqref="J174"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2670,7 +2670,7 @@
         <v>109</v>
       </c>
       <c r="C174" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E174" s="38" t="s">
         <v>115</v>
@@ -2710,11 +2710,11 @@
       </c>
       <c r="C178" s="19">
         <f>SUM(C174:C177)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E178" s="41">
         <f>C178*40000</f>
-        <v>760000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="179" spans="2:5" x14ac:dyDescent="0.3">
@@ -2722,7 +2722,7 @@
         <v>2</v>
       </c>
       <c r="D179" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>